<commit_message>
fix: fixes a bug
</commit_message>
<xml_diff>
--- a/follow_students/static/excel_format/FORMATO_IBQ_CURSOS-NOTAS.xlsx
+++ b/follow_students/static/excel_format/FORMATO_IBQ_CURSOS-NOTAS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icesiedu-my.sharepoint.com/personal/1107835369_u_icesi_edu_co/Documents/Quinto semestre/Proyecto Integrador/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/662df145e42404a6/Semestre5/Final-Project/follow_students/static/excel_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="12" documentId="8_{CB7B0996-492C-4FA2-8B36-45C113585027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E6D04A5-08B2-4B7C-A680-00E4B4A1040C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="54" xr2:uid="{37C6A70E-0892-4DA6-B95F-1D86B2DF07FB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="5" xr2:uid="{37C6A70E-0892-4DA6-B95F-1D86B2DF07FB}"/>
   </bookViews>
   <sheets>
     <sheet name="_x0009_MAT-08273" sheetId="2" r:id="rId1"/>
@@ -614,17 +614,17 @@
       <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -634,7 +634,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -644,7 +644,7 @@
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -654,7 +654,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -664,7 +664,7 @@
       <c r="C5" s="3"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -674,7 +674,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -684,7 +684,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -694,7 +694,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -704,7 +704,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -714,7 +714,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -724,7 +724,7 @@
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -734,7 +734,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -744,7 +744,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -754,7 +754,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -764,7 +764,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -774,7 +774,7 @@
       <c r="C16" s="3"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="C17" s="3"/>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -794,7 +794,7 @@
       <c r="C18" s="3"/>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -804,7 +804,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -814,7 +814,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -824,7 +824,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -834,7 +834,7 @@
       <c r="C22" s="3"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -844,7 +844,7 @@
       <c r="C23" s="3"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -854,7 +854,7 @@
       <c r="C24" s="3"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -864,7 +864,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -874,7 +874,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -884,7 +884,7 @@
       <c r="C27" s="3"/>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -894,7 +894,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -904,7 +904,7 @@
       <c r="C29" s="3"/>
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -914,7 +914,7 @@
       <c r="C30" s="3"/>
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -924,7 +924,7 @@
       <c r="C31" s="3"/>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -934,7 +934,7 @@
       <c r="C32" s="3"/>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -944,7 +944,7 @@
       <c r="C33" s="3"/>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -954,7 +954,7 @@
       <c r="C34" s="3"/>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -964,7 +964,7 @@
       <c r="C35" s="3"/>
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -974,7 +974,7 @@
       <c r="C36" s="3"/>
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -984,7 +984,7 @@
       <c r="C37" s="3"/>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -1007,9 +1007,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1030,9 +1030,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1053,9 +1053,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1074,7 +1074,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1088,9 +1088,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1111,9 +1111,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1134,9 +1134,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1157,9 +1157,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1180,9 +1180,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1203,9 +1203,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1226,17 +1226,17 @@
       <selection activeCell="B2" sqref="B2:B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1246,7 +1246,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1256,7 +1256,7 @@
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1266,7 +1266,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1276,7 +1276,7 @@
       <c r="C5" s="3"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1286,7 +1286,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1296,7 +1296,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1306,7 +1306,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1316,7 +1316,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1326,7 +1326,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1336,7 +1336,7 @@
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1346,7 +1346,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1366,7 +1366,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1376,7 +1376,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1386,7 +1386,7 @@
       <c r="C16" s="3"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1396,7 +1396,7 @@
       <c r="C17" s="3"/>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1406,7 +1406,7 @@
       <c r="C18" s="3"/>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1416,7 +1416,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1426,7 +1426,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1436,7 +1436,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1446,7 +1446,7 @@
       <c r="C22" s="3"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1456,7 +1456,7 @@
       <c r="C23" s="3"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1466,7 +1466,7 @@
       <c r="C24" s="3"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1476,7 +1476,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1486,7 +1486,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1496,7 +1496,7 @@
       <c r="C27" s="3"/>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1506,7 +1506,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1516,7 +1516,7 @@
       <c r="C29" s="3"/>
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1526,7 +1526,7 @@
       <c r="C30" s="3"/>
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -1536,7 +1536,7 @@
       <c r="C31" s="3"/>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -1546,7 +1546,7 @@
       <c r="C32" s="3"/>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -1556,7 +1556,7 @@
       <c r="C33" s="3"/>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -1566,7 +1566,7 @@
       <c r="C34" s="3"/>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -1576,7 +1576,7 @@
       <c r="C35" s="3"/>
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="C36" s="3"/>
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -1596,7 +1596,7 @@
       <c r="C37" s="3"/>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -1618,7 +1618,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1632,9 +1632,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1655,9 +1655,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1678,9 +1678,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1701,9 +1701,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1724,9 +1724,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1747,7 +1747,7 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1761,9 +1761,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1784,9 +1784,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1807,9 +1807,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1830,17 +1830,17 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>1.62</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -2149,9 +2149,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2172,9 +2172,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2195,9 +2195,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2216,7 +2216,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2230,9 +2230,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2253,9 +2253,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2276,9 +2276,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2299,9 +2299,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2322,9 +2322,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2345,9 +2345,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2368,17 +2368,17 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>1.62</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -2610,7 +2610,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -2650,7 +2650,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -2685,7 +2685,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2699,9 +2699,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2722,9 +2722,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2745,9 +2745,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2768,9 +2768,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2791,9 +2791,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2814,9 +2814,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2835,7 +2835,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2849,9 +2849,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2872,9 +2872,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2895,17 +2895,17 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>1.62</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -3214,9 +3214,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3237,9 +3237,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3260,9 +3260,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3283,9 +3283,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3306,9 +3306,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3325,13 +3325,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0737EFB5-3DFE-4D77-B716-ECE083F24D03}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
     </row>
@@ -3348,9 +3348,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3371,9 +3371,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3394,9 +3394,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3417,9 +3417,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3436,21 +3436,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C0C75F-C9B6-4BCF-ABB9-B7B70F863CE0}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>1.17</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>1.62</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>1.73</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -3658,7 +3658,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -3690,7 +3690,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -3715,7 +3715,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -3760,9 +3760,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3783,9 +3783,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3806,9 +3806,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3827,7 +3827,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3841,9 +3841,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3864,7 +3864,7 @@
       <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3878,9 +3878,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3901,9 +3901,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>